<commit_message>
Updated to latest version/ files
</commit_message>
<xml_diff>
--- a/Mean_RGDP_Level.xlsx
+++ b/Mean_RGDP_Level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b09e99cea646701/Bloomberg/Projects/FOMC/FOMC Paper/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{FF4161F5-2282-4523-BA38-DAF215EECFD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6851B7D3-2579-4FEF-8BA4-C45BA5C62334}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{FF4161F5-2282-4523-BA38-DAF215EECFD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C89B42D4-4094-4675-A754-F7EF0D63DDD7}"/>
   <bookViews>
-    <workbookView xWindow="11016" yWindow="600" windowWidth="13584" windowHeight="13524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean_Level" sheetId="1" r:id="rId1"/>
@@ -76,10 +76,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="##0"/>
+    <numFmt numFmtId="169" formatCode="0.000000%"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,6 +95,10 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="ITC Bookman"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="ITC Bookman"/>
     </font>
   </fonts>
@@ -124,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -140,10 +145,16 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -283,8 +294,8 @@
   <dimension ref="A1:L211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C213" sqref="C213:E214"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D211" sqref="D211:E211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.05" customHeight="1"/>
@@ -5164,7 +5175,7 @@
       <c r="B129" s="3">
         <v>3</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C129" s="4">
         <v>9308.7999999999993</v>
       </c>
       <c r="D129" s="4">
@@ -8198,22 +8209,22 @@
       </c>
     </row>
     <row r="209" spans="1:12" ht="15" customHeight="1">
-      <c r="A209" s="3">
+      <c r="A209" s="6">
         <v>2020</v>
       </c>
-      <c r="B209" s="3">
+      <c r="B209" s="6">
         <v>3</v>
       </c>
-      <c r="C209" s="4">
+      <c r="C209" s="7">
         <v>17205.8007</v>
       </c>
-      <c r="D209" s="4">
+      <c r="D209" s="7">
         <v>17981.5416</v>
       </c>
-      <c r="E209" s="4">
+      <c r="E209" s="7">
         <v>18224.003499999999</v>
       </c>
-      <c r="F209" s="4">
+      <c r="F209" s="7">
         <v>18431.249400000001</v>
       </c>
       <c r="G209" s="4">
@@ -8274,11 +8285,11 @@
       </c>
     </row>
     <row r="211" spans="1:12" ht="13.05" customHeight="1">
-      <c r="D211" s="6"/>
-      <c r="E211" s="6"/>
-      <c r="F211" s="6"/>
-      <c r="G211" s="6"/>
-      <c r="H211" s="6"/>
+      <c r="D211" s="8"/>
+      <c r="E211" s="8"/>
+      <c r="F211" s="5"/>
+      <c r="G211" s="5"/>
+      <c r="H211" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>